<commit_message>
code running beforeupdating climate sensitivity spreadsheet and parameters. updated upper to central (190USD) using epa docs.
</commit_message>
<xml_diff>
--- a/cmu_tare_model/data/marginal_social_costs/scc_climate_impact_sensitivity.xlsx
+++ b/cmu_tare_model/data/marginal_social_costs/scc_climate_impact_sensitivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\cmu_tare_model\public_impact\data_processing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\cmu_tare_model\data\marginal_social_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{494B9539-34DA-447E-A8D5-E2EE3200148D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A7AA3-D9BE-43A0-B8A4-FE686F117240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{9E84D423-0E0D-4820-8255-FAB67149DDA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{9E84D423-0E0D-4820-8255-FAB67149DDA4}"/>
   </bookViews>
   <sheets>
     <sheet name="scc_lower" sheetId="1" r:id="rId1"/>
@@ -213,22 +213,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>22860</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>198558</xdr:colOff>
+      <xdr:colOff>183318</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>99273</xdr:rowOff>
+      <xdr:rowOff>30693</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="6" name="Group 5">
+        <xdr:cNvPr id="2" name="Group 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A2B0E56-198B-62C2-9485-FFA397D8861C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBA756E9-337A-47F3-B5F7-538E576BB100}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -236,18 +236,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6143625" y="762000"/>
-          <a:ext cx="5058213" cy="2429088"/>
-          <a:chOff x="6065520" y="38100"/>
+          <a:off x="6233160" y="701040"/>
+          <a:ext cx="5052498" cy="2453853"/>
+          <a:chOff x="6233160" y="701040"/>
           <a:chExt cx="5052498" cy="2453853"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="Picture 3">
+          <xdr:cNvPr id="3" name="Picture 2">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{826FB55C-2A89-44D4-97F7-8DC97D500D27}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BFE6072-FFBC-C7F8-6AB1-5EA70580EED9}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -269,7 +269,7 @@
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6065520" y="38100"/>
+            <a:off x="6233160" y="701040"/>
             <a:ext cx="5052498" cy="2453853"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -279,10 +279,10 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Rectangle 4">
+          <xdr:cNvPr id="7" name="Rectangle 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{353A723A-2443-4042-A310-4D2B3664CB5A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8612FE2B-D323-4C97-6D2D-8A6634D4D41F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -290,7 +290,7 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="7459980" y="746760"/>
+            <a:off x="8412480" y="1417320"/>
             <a:ext cx="624840" cy="1577340"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
@@ -339,22 +339,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>183318</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>30693</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>274869</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>91637</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="4" name="Group 3">
+        <xdr:cNvPr id="5" name="Group 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59873BD4-486E-D0DE-72F8-77785FFC26E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD92BEDD-C352-4B75-8E16-7A60E0F14608}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -362,18 +362,18 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6238875" y="695325"/>
-          <a:ext cx="5048688" cy="2429088"/>
-          <a:chOff x="6233160" y="701040"/>
-          <a:chExt cx="5052498" cy="2453853"/>
+          <a:off x="6156960" y="762000"/>
+          <a:ext cx="6332769" cy="2270957"/>
+          <a:chOff x="5913120" y="137160"/>
+          <a:chExt cx="6332769" cy="2270957"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:pic>
         <xdr:nvPicPr>
-          <xdr:cNvPr id="2" name="Picture 1">
+          <xdr:cNvPr id="6" name="Picture 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9E12E2-951F-4B4C-993B-4D7456B38226}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8964B44-6AAE-BB25-E7CD-ADC18635FE7A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -395,8 +395,8 @@
         </xdr:blipFill>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="6233160" y="701040"/>
-            <a:ext cx="5052498" cy="2453853"/>
+            <a:off x="5913120" y="137160"/>
+            <a:ext cx="6332769" cy="2270957"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -405,10 +405,10 @@
       </xdr:pic>
       <xdr:sp macro="" textlink="">
         <xdr:nvSpPr>
-          <xdr:cNvPr id="3" name="Rectangle 2">
+          <xdr:cNvPr id="7" name="Rectangle 6">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD082A4E-12EB-449A-8773-E69B263E365A}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85D948DA-DF1F-5B98-095B-8269A99759B4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -416,8 +416,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="8412480" y="1417320"/>
-            <a:ext cx="624840" cy="1577340"/>
+            <a:off x="9174480" y="1005840"/>
+            <a:ext cx="502920" cy="1348740"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -488,8 +488,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6162675" y="762000"/>
-          <a:ext cx="6334674" cy="2248097"/>
+          <a:off x="6156960" y="762000"/>
+          <a:ext cx="6332769" cy="2270957"/>
           <a:chOff x="5913120" y="137160"/>
           <a:chExt cx="6332769" cy="2270957"/>
         </a:xfrm>
@@ -905,375 +905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EC15B2-2397-4FE1-8B68-09BFA0B5EF94}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="16.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2020</v>
-      </c>
-      <c r="B2">
-        <v>14</v>
-      </c>
-      <c r="D2">
-        <v>2020</v>
-      </c>
-      <c r="E2" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D2,$B$2:$B$3,$A$2:$A$3)</f>
-        <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2025</v>
-      </c>
-      <c r="B3">
-        <v>17</v>
-      </c>
-      <c r="D3">
-        <v>2021</v>
-      </c>
-      <c r="E3" s="2">
-        <f t="shared" ref="E3:E7" si="0">_xlfn.FORECAST.LINEAR(D3,$B$2:$B$3,$A$2:$A$3)</f>
-        <v>14.599999999999909</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2030</v>
-      </c>
-      <c r="B4">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>2022</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="0"/>
-        <v>15.200000000000045</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2035</v>
-      </c>
-      <c r="B5">
-        <v>22</v>
-      </c>
-      <c r="D5">
-        <v>2023</v>
-      </c>
-      <c r="E5" s="2">
-        <f t="shared" si="0"/>
-        <v>15.799999999999955</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2040</v>
-      </c>
-      <c r="B6">
-        <v>25</v>
-      </c>
-      <c r="D6">
-        <v>2024</v>
-      </c>
-      <c r="E6" s="2">
-        <f t="shared" si="0"/>
-        <v>16.399999999999864</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2045</v>
-      </c>
-      <c r="B7">
-        <v>28</v>
-      </c>
-      <c r="D7">
-        <v>2025</v>
-      </c>
-      <c r="E7" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2050</v>
-      </c>
-      <c r="B8">
-        <v>32</v>
-      </c>
-      <c r="D8">
-        <v>2026</v>
-      </c>
-      <c r="E8" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D8,$B$3:$B$4,$A$3:$A$4)</f>
-        <v>17.400000000000091</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D9">
-        <v>2027</v>
-      </c>
-      <c r="E9" s="2">
-        <f t="shared" ref="E9:E12" si="1">_xlfn.FORECAST.LINEAR(D9,$B$3:$B$4,$A$3:$A$4)</f>
-        <v>17.800000000000068</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D10">
-        <v>2028</v>
-      </c>
-      <c r="E10" s="2">
-        <f t="shared" si="1"/>
-        <v>18.200000000000045</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D11">
-        <v>2029</v>
-      </c>
-      <c r="E11" s="2">
-        <f t="shared" si="1"/>
-        <v>18.600000000000023</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D12">
-        <v>2030</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="1"/>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D13">
-        <v>2031</v>
-      </c>
-      <c r="E13" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D13,$B$4:$B$5,$A$4:$A$5)</f>
-        <v>19.599999999999909</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D14">
-        <v>2032</v>
-      </c>
-      <c r="E14" s="2">
-        <f t="shared" ref="E14:E17" si="2">_xlfn.FORECAST.LINEAR(D14,$B$4:$B$5,$A$4:$A$5)</f>
-        <v>20.200000000000045</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D15">
-        <v>2033</v>
-      </c>
-      <c r="E15" s="2">
-        <f t="shared" si="2"/>
-        <v>20.799999999999955</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="D16">
-        <v>2034</v>
-      </c>
-      <c r="E16" s="2">
-        <f t="shared" si="2"/>
-        <v>21.399999999999864</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17">
-        <v>2035</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D18">
-        <v>2036</v>
-      </c>
-      <c r="E18" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D18,$B$5:$B$6,$A$5:$A$6)</f>
-        <v>22.599999999999909</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D19">
-        <v>2037</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" ref="E19:E22" si="3">_xlfn.FORECAST.LINEAR(D19,$B$5:$B$6,$A$5:$A$6)</f>
-        <v>23.200000000000045</v>
-      </c>
-    </row>
-    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D20">
-        <v>2038</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="3"/>
-        <v>23.799999999999955</v>
-      </c>
-    </row>
-    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D21">
-        <v>2039</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="3"/>
-        <v>24.399999999999864</v>
-      </c>
-    </row>
-    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D22">
-        <v>2040</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="3"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D23">
-        <v>2041</v>
-      </c>
-      <c r="E23" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D23,$B$6:$B$7,$A$6:$A$7)</f>
-        <v>25.599999999999909</v>
-      </c>
-    </row>
-    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D24">
-        <v>2042</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" ref="E24:E27" si="4">_xlfn.FORECAST.LINEAR(D24,$B$6:$B$7,$A$6:$A$7)</f>
-        <v>26.200000000000045</v>
-      </c>
-    </row>
-    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D25">
-        <v>2043</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="4"/>
-        <v>26.799999999999955</v>
-      </c>
-    </row>
-    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D26">
-        <v>2044</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="4"/>
-        <v>27.399999999999864</v>
-      </c>
-    </row>
-    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D27">
-        <v>2045</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="4"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D28">
-        <v>2046</v>
-      </c>
-      <c r="E28" s="2">
-        <f>_xlfn.FORECAST.LINEAR(D28,$B$7:$B$8,$A$7:$A$8)</f>
-        <v>28.800000000000182</v>
-      </c>
-    </row>
-    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D29">
-        <v>2047</v>
-      </c>
-      <c r="E29" s="2">
-        <f t="shared" ref="E29:E32" si="5">_xlfn.FORECAST.LINEAR(D29,$B$7:$B$8,$A$7:$A$8)</f>
-        <v>29.600000000000136</v>
-      </c>
-    </row>
-    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D30">
-        <v>2048</v>
-      </c>
-      <c r="E30" s="2">
-        <f t="shared" si="5"/>
-        <v>30.400000000000091</v>
-      </c>
-    </row>
-    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D31">
-        <v>2049</v>
-      </c>
-      <c r="E31" s="2">
-        <f t="shared" si="5"/>
-        <v>31.200000000000045</v>
-      </c>
-    </row>
-    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D32">
-        <v>2050</v>
-      </c>
-      <c r="E32" s="2">
-        <f t="shared" si="5"/>
-        <v>32</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2851B3AE-E1A0-40CD-8D9C-3E7FD3B3E981}">
-  <dimension ref="A1:H32"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,13 +922,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1637,12 +1270,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754CFF6-6F51-4025-99D4-87B6BEDCE997}">
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2851B3AE-E1A0-40CD-8D9C-3E7FD3B3E981}">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1658,13 +1291,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1980,6 +1613,357 @@
       <c r="E32" s="2">
         <f t="shared" si="2"/>
         <v>290</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754CFF6-6F51-4025-99D4-87B6BEDCE997}">
+  <dimension ref="A1:H32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="21.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>310</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" s="2">
+        <f>_xlfn.FORECAST.LINEAR(D2,$B$2:$B$3,$A$2:$A$3)</f>
+        <v>310</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2030</v>
+      </c>
+      <c r="B3">
+        <v>350</v>
+      </c>
+      <c r="D3">
+        <v>2021</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E12" si="0">_xlfn.FORECAST.LINEAR(D3,$B$2:$B$3,$A$2:$A$3)</f>
+        <v>314</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>2040</v>
+      </c>
+      <c r="B4">
+        <v>390</v>
+      </c>
+      <c r="D4">
+        <v>2022</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2050</v>
+      </c>
+      <c r="B5">
+        <v>430</v>
+      </c>
+      <c r="D5">
+        <v>2023</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D6">
+        <v>2024</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D7">
+        <v>2025</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D8">
+        <v>2026</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D9">
+        <v>2027</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D10">
+        <v>2028</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>342</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D11">
+        <v>2029</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D12">
+        <v>2030</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>350</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D13">
+        <v>2031</v>
+      </c>
+      <c r="E13" s="2">
+        <f>_xlfn.FORECAST.LINEAR(D13,$B$3:$B$4,$A$3:$A$4)</f>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D14">
+        <v>2032</v>
+      </c>
+      <c r="E14" s="2">
+        <f t="shared" ref="E14:E22" si="1">_xlfn.FORECAST.LINEAR(D14,$B$3:$B$4,$A$3:$A$4)</f>
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D15">
+        <v>2033</v>
+      </c>
+      <c r="E15" s="2">
+        <f t="shared" si="1"/>
+        <v>362</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D16">
+        <v>2034</v>
+      </c>
+      <c r="E16" s="2">
+        <f t="shared" si="1"/>
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17">
+        <v>2035</v>
+      </c>
+      <c r="E17" s="2">
+        <f t="shared" si="1"/>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="18" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D18">
+        <v>2036</v>
+      </c>
+      <c r="E18" s="2">
+        <f t="shared" si="1"/>
+        <v>374</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19">
+        <v>2037</v>
+      </c>
+      <c r="E19" s="2">
+        <f t="shared" si="1"/>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D20">
+        <v>2038</v>
+      </c>
+      <c r="E20" s="2">
+        <f t="shared" si="1"/>
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D21">
+        <v>2039</v>
+      </c>
+      <c r="E21" s="2">
+        <f t="shared" si="1"/>
+        <v>386</v>
+      </c>
+    </row>
+    <row r="22" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D22">
+        <v>2040</v>
+      </c>
+      <c r="E22" s="2">
+        <f t="shared" si="1"/>
+        <v>390</v>
+      </c>
+    </row>
+    <row r="23" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D23">
+        <v>2041</v>
+      </c>
+      <c r="E23" s="2">
+        <f>_xlfn.FORECAST.LINEAR(D23,$B$4:$B$5,$A$4:$A$5)</f>
+        <v>394</v>
+      </c>
+    </row>
+    <row r="24" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D24">
+        <v>2042</v>
+      </c>
+      <c r="E24" s="2">
+        <f t="shared" ref="E24:E32" si="2">_xlfn.FORECAST.LINEAR(D24,$B$4:$B$5,$A$4:$A$5)</f>
+        <v>398</v>
+      </c>
+    </row>
+    <row r="25" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D25">
+        <v>2043</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="2"/>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="26" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D26">
+        <v>2044</v>
+      </c>
+      <c r="E26" s="2">
+        <f t="shared" si="2"/>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="27" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D27">
+        <v>2045</v>
+      </c>
+      <c r="E27" s="2">
+        <f t="shared" si="2"/>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="28" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D28">
+        <v>2046</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="2"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="29" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D29">
+        <v>2047</v>
+      </c>
+      <c r="E29" s="2">
+        <f t="shared" si="2"/>
+        <v>418</v>
+      </c>
+    </row>
+    <row r="30" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D30">
+        <v>2048</v>
+      </c>
+      <c r="E30" s="2">
+        <f t="shared" si="2"/>
+        <v>422</v>
+      </c>
+    </row>
+    <row r="31" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D31">
+        <v>2049</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="2"/>
+        <v>426</v>
+      </c>
+    </row>
+    <row r="32" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D32">
+        <v>2050</v>
+      </c>
+      <c r="E32" s="2">
+        <f t="shared" si="2"/>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +1976,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B38A36-4C8F-4743-A26E-038C2421567B}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2040,28 +2026,28 @@
         <v>2020</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="C2">
-        <v>51</v>
+        <v>190</v>
       </c>
       <c r="D2">
-        <v>190</v>
+        <v>310</v>
       </c>
       <c r="E2">
         <v>1.1773147200080301</v>
       </c>
       <c r="F2" s="1">
         <f>$B2*$E2</f>
-        <v>16.482406080112419</v>
+        <v>60.043050720409532</v>
       </c>
       <c r="G2" s="1">
         <f>$C2*$E2</f>
-        <v>60.043050720409532</v>
+        <v>223.68979680152572</v>
       </c>
       <c r="H2" s="1">
         <f>$D2*$E2</f>
-        <v>223.68979680152572</v>
+        <v>364.96756320248932</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -2069,28 +2055,28 @@
         <v>2021</v>
       </c>
       <c r="B3">
-        <v>14.599999999999909</v>
+        <v>52</v>
       </c>
       <c r="C3">
-        <v>52</v>
+        <v>193</v>
       </c>
       <c r="D3">
-        <v>193</v>
+        <v>314</v>
       </c>
       <c r="E3">
         <v>1.1773147200080301</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F32" si="0">$B3*$E3</f>
-        <v>17.188794912117132</v>
+        <v>61.220365440417567</v>
       </c>
       <c r="G3" s="1">
         <f t="shared" ref="G3:G32" si="1">$C3*$E3</f>
-        <v>61.220365440417567</v>
+        <v>227.22174096154981</v>
       </c>
       <c r="H3" s="1">
         <f t="shared" ref="H3:H32" si="2">$D3*$E3</f>
-        <v>227.22174096154981</v>
+        <v>369.67682208252143</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2098,28 +2084,28 @@
         <v>2022</v>
       </c>
       <c r="B4">
-        <v>15.200000000000045</v>
+        <v>53</v>
       </c>
       <c r="C4">
-        <v>53</v>
+        <v>196</v>
       </c>
       <c r="D4">
-        <v>196</v>
+        <v>318</v>
       </c>
       <c r="E4">
         <v>1.1773147200080301</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>17.895183744122111</v>
+        <v>62.397680160425594</v>
       </c>
       <c r="G4" s="1">
         <f t="shared" si="1"/>
-        <v>62.397680160425594</v>
+        <v>230.75368512157388</v>
       </c>
       <c r="H4" s="1">
         <f t="shared" si="2"/>
-        <v>230.75368512157388</v>
+        <v>374.38608096255354</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2127,28 +2113,28 @@
         <v>2023</v>
       </c>
       <c r="B5">
-        <v>15.799999999999955</v>
+        <v>54</v>
       </c>
       <c r="C5">
-        <v>54</v>
+        <v>199</v>
       </c>
       <c r="D5">
-        <v>199</v>
+        <v>322</v>
       </c>
       <c r="E5">
         <v>1.1773147200080301</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>18.60157257612682</v>
+        <v>63.574994880433621</v>
       </c>
       <c r="G5" s="1">
         <f t="shared" si="1"/>
-        <v>63.574994880433621</v>
+        <v>234.28562928159798</v>
       </c>
       <c r="H5" s="1">
         <f t="shared" si="2"/>
-        <v>234.28562928159798</v>
+        <v>379.0953398425857</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -2156,28 +2142,28 @@
         <v>2024</v>
       </c>
       <c r="B6">
-        <v>16.399999999999864</v>
+        <v>55</v>
       </c>
       <c r="C6">
-        <v>55</v>
+        <v>202</v>
       </c>
       <c r="D6">
-        <v>202</v>
+        <v>326</v>
       </c>
       <c r="E6">
         <v>1.1773147200080301</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>19.307961408131533</v>
+        <v>64.752309600441649</v>
       </c>
       <c r="G6" s="1">
         <f t="shared" si="1"/>
-        <v>64.752309600441649</v>
+        <v>237.81757344162207</v>
       </c>
       <c r="H6" s="1">
         <f t="shared" si="2"/>
-        <v>237.81757344162207</v>
+        <v>383.80459872261781</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2185,28 +2171,28 @@
         <v>2025</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="C7">
-        <v>56</v>
+        <v>205</v>
       </c>
       <c r="D7">
-        <v>205</v>
+        <v>330</v>
       </c>
       <c r="E7">
         <v>1.1773147200080301</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>20.014350240136512</v>
+        <v>65.929624320449676</v>
       </c>
       <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>65.929624320449676</v>
+        <v>241.34951760164617</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" si="2"/>
-        <v>241.34951760164617</v>
+        <v>388.51385760264992</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2214,28 +2200,28 @@
         <v>2026</v>
       </c>
       <c r="B8">
-        <v>17.400000000000091</v>
+        <v>57.199999999999818</v>
       </c>
       <c r="C8">
-        <v>57.199999999999818</v>
+        <v>208</v>
       </c>
       <c r="D8">
-        <v>208</v>
+        <v>334</v>
       </c>
       <c r="E8">
         <v>1.1773147200080301</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>20.48527612813983</v>
+        <v>67.342401984459102</v>
       </c>
       <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>67.342401984459102</v>
+        <v>244.88146176167027</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="2"/>
-        <v>244.88146176167027</v>
+        <v>393.22311648268203</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -2243,28 +2229,28 @@
         <v>2027</v>
       </c>
       <c r="B9">
-        <v>17.800000000000068</v>
+        <v>58.400000000000091</v>
       </c>
       <c r="C9">
-        <v>58.400000000000091</v>
+        <v>211</v>
       </c>
       <c r="D9">
-        <v>211</v>
+        <v>338</v>
       </c>
       <c r="E9">
         <v>1.1773147200080301</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>20.956202016143017</v>
+        <v>68.755179648469067</v>
       </c>
       <c r="G9" s="1">
         <f t="shared" si="1"/>
-        <v>68.755179648469067</v>
+        <v>248.41340592169433</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="2"/>
-        <v>248.41340592169433</v>
+        <v>397.93237536271414</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -2272,28 +2258,28 @@
         <v>2028</v>
       </c>
       <c r="B10">
-        <v>18.200000000000045</v>
+        <v>59.599999999999909</v>
       </c>
       <c r="C10">
-        <v>59.599999999999909</v>
+        <v>214</v>
       </c>
       <c r="D10">
-        <v>214</v>
+        <v>342</v>
       </c>
       <c r="E10">
         <v>1.1773147200080301</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>21.4271279041462</v>
+        <v>70.167957312478478</v>
       </c>
       <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>70.167957312478478</v>
+        <v>251.94535008171843</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="2"/>
-        <v>251.94535008171843</v>
+        <v>402.64163424274631</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -2301,28 +2287,28 @@
         <v>2029</v>
       </c>
       <c r="B11">
-        <v>18.600000000000023</v>
+        <v>60.799999999999727</v>
       </c>
       <c r="C11">
-        <v>60.799999999999727</v>
+        <v>217</v>
       </c>
       <c r="D11">
-        <v>217</v>
+        <v>346</v>
       </c>
       <c r="E11">
         <v>1.1773147200080301</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>21.898053792149387</v>
+        <v>71.580734976487904</v>
       </c>
       <c r="G11" s="1">
         <f t="shared" si="1"/>
-        <v>71.580734976487904</v>
+        <v>255.47729424174253</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="2"/>
-        <v>255.47729424174253</v>
+        <v>407.35089312277842</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -2330,28 +2316,28 @@
         <v>2030</v>
       </c>
       <c r="B12">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="C12">
-        <v>62</v>
+        <v>220</v>
       </c>
       <c r="D12">
-        <v>220</v>
+        <v>350</v>
       </c>
       <c r="E12">
         <v>1.1773147200080301</v>
       </c>
       <c r="F12" s="1">
         <f>$B12*$E12</f>
-        <v>22.36897968015257</v>
+        <v>72.993512640497869</v>
       </c>
       <c r="G12" s="1">
         <f t="shared" si="1"/>
-        <v>72.993512640497869</v>
+        <v>259.00923840176659</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="2"/>
-        <v>259.00923840176659</v>
+        <v>412.06015200281053</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2359,28 +2345,28 @@
         <v>2031</v>
       </c>
       <c r="B13">
-        <v>19.599999999999909</v>
+        <v>63</v>
       </c>
       <c r="C13">
-        <v>63</v>
+        <v>223</v>
       </c>
       <c r="D13">
-        <v>223</v>
+        <v>354</v>
       </c>
       <c r="E13">
         <v>1.1773147200080301</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>23.075368512157283</v>
+        <v>74.170827360505896</v>
       </c>
       <c r="G13" s="1">
         <f t="shared" si="1"/>
-        <v>74.170827360505896</v>
+        <v>262.54118256179072</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="2"/>
-        <v>262.54118256179072</v>
+        <v>416.76941088284264</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -2388,28 +2374,28 @@
         <v>2032</v>
       </c>
       <c r="B14">
-        <v>20.200000000000045</v>
+        <v>64</v>
       </c>
       <c r="C14">
-        <v>64</v>
+        <v>226</v>
       </c>
       <c r="D14">
-        <v>226</v>
+        <v>358</v>
       </c>
       <c r="E14">
         <v>1.1773147200080301</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>23.781757344162262</v>
+        <v>75.348142080513924</v>
       </c>
       <c r="G14" s="1">
         <f t="shared" si="1"/>
-        <v>75.348142080513924</v>
+        <v>266.07312672181479</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="2"/>
-        <v>266.07312672181479</v>
+        <v>421.47866976287474</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2417,28 +2403,28 @@
         <v>2033</v>
       </c>
       <c r="B15">
-        <v>20.799999999999955</v>
+        <v>65</v>
       </c>
       <c r="C15">
-        <v>65</v>
+        <v>229</v>
       </c>
       <c r="D15">
-        <v>229</v>
+        <v>362</v>
       </c>
       <c r="E15">
         <v>1.1773147200080301</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>24.488146176166971</v>
+        <v>76.525456800521951</v>
       </c>
       <c r="G15" s="1">
         <f t="shared" si="1"/>
-        <v>76.525456800521951</v>
+        <v>269.60507088183886</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="2"/>
-        <v>269.60507088183886</v>
+        <v>426.18792864290685</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2446,28 +2432,28 @@
         <v>2034</v>
       </c>
       <c r="B16">
-        <v>21.399999999999864</v>
+        <v>66</v>
       </c>
       <c r="C16">
-        <v>66</v>
+        <v>232</v>
       </c>
       <c r="D16">
-        <v>232</v>
+        <v>366</v>
       </c>
       <c r="E16">
         <v>1.1773147200080301</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>25.194535008171684</v>
+        <v>77.702771520529978</v>
       </c>
       <c r="G16" s="1">
         <f t="shared" si="1"/>
-        <v>77.702771520529978</v>
+        <v>273.13701504186298</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="2"/>
-        <v>273.13701504186298</v>
+        <v>430.89718752293902</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -2475,28 +2461,28 @@
         <v>2035</v>
       </c>
       <c r="B17">
-        <v>22</v>
+        <v>67</v>
       </c>
       <c r="C17">
-        <v>67</v>
+        <v>235</v>
       </c>
       <c r="D17">
-        <v>235</v>
+        <v>370</v>
       </c>
       <c r="E17">
         <v>1.1773147200080301</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>25.900923840176659</v>
+        <v>78.88008624053802</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="1"/>
-        <v>78.88008624053802</v>
+        <v>276.66895920188705</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="2"/>
-        <v>276.66895920188705</v>
+        <v>435.60644640297113</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -2504,28 +2490,28 @@
         <v>2036</v>
       </c>
       <c r="B18">
-        <v>22.599999999999909</v>
+        <v>68.199999999999818</v>
       </c>
       <c r="C18">
-        <v>68.199999999999818</v>
+        <v>238</v>
       </c>
       <c r="D18">
-        <v>238</v>
+        <v>374</v>
       </c>
       <c r="E18">
         <v>1.1773147200080301</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>26.607312672181372</v>
+        <v>80.292863904547431</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="1"/>
-        <v>80.292863904547431</v>
+        <v>280.20090336191117</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="2"/>
-        <v>280.20090336191117</v>
+        <v>440.31570528300324</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -2533,28 +2519,28 @@
         <v>2037</v>
       </c>
       <c r="B19">
-        <v>23.200000000000045</v>
+        <v>69.400000000000091</v>
       </c>
       <c r="C19">
-        <v>69.400000000000091</v>
+        <v>241</v>
       </c>
       <c r="D19">
-        <v>241</v>
+        <v>378</v>
       </c>
       <c r="E19">
         <v>1.1773147200080301</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>27.313701504186351</v>
+        <v>81.705641568557397</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="1"/>
-        <v>81.705641568557397</v>
+        <v>283.73284752193524</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="2"/>
-        <v>283.73284752193524</v>
+        <v>445.02496416303535</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -2562,28 +2548,28 @@
         <v>2038</v>
       </c>
       <c r="B20">
-        <v>23.799999999999955</v>
+        <v>70.599999999999909</v>
       </c>
       <c r="C20">
-        <v>70.599999999999909</v>
+        <v>244</v>
       </c>
       <c r="D20">
-        <v>244</v>
+        <v>382</v>
       </c>
       <c r="E20">
         <v>1.1773147200080301</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>28.02009033619106</v>
+        <v>83.118419232566822</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="1"/>
-        <v>83.118419232566822</v>
+        <v>287.26479168195931</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="2"/>
-        <v>287.26479168195931</v>
+        <v>449.73422304306746</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -2591,28 +2577,28 @@
         <v>2039</v>
       </c>
       <c r="B21">
-        <v>24.399999999999864</v>
+        <v>71.799999999999727</v>
       </c>
       <c r="C21">
-        <v>71.799999999999727</v>
+        <v>247</v>
       </c>
       <c r="D21">
-        <v>247</v>
+        <v>386</v>
       </c>
       <c r="E21">
         <v>1.1773147200080301</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>28.726479168195773</v>
+        <v>84.531196896576233</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="1"/>
-        <v>84.531196896576233</v>
+        <v>290.79673584198343</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="2"/>
-        <v>290.79673584198343</v>
+        <v>454.44348192309963</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -2620,28 +2606,28 @@
         <v>2040</v>
       </c>
       <c r="B22">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C22">
-        <v>73</v>
+        <v>250</v>
       </c>
       <c r="D22">
-        <v>250</v>
+        <v>390</v>
       </c>
       <c r="E22">
         <v>1.1773147200080301</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>29.432868000200752</v>
+        <v>85.943974560586199</v>
       </c>
       <c r="G22" s="1">
         <f t="shared" si="1"/>
-        <v>85.943974560586199</v>
+        <v>294.3286800020075</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="2"/>
-        <v>294.3286800020075</v>
+        <v>459.15274080313173</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -2649,28 +2635,28 @@
         <v>2041</v>
       </c>
       <c r="B23">
-        <v>25.599999999999909</v>
+        <v>74.199999999999818</v>
       </c>
       <c r="C23">
-        <v>74.199999999999818</v>
+        <v>254</v>
       </c>
       <c r="D23">
-        <v>254</v>
+        <v>394</v>
       </c>
       <c r="E23">
         <v>1.1773147200080301</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>30.139256832205461</v>
+        <v>87.35675222459561</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="1"/>
-        <v>87.35675222459561</v>
+        <v>299.03793888203961</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="2"/>
-        <v>299.03793888203961</v>
+        <v>463.86199968316384</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -2678,28 +2664,28 @@
         <v>2042</v>
       </c>
       <c r="B24">
-        <v>26.200000000000045</v>
+        <v>75.400000000000091</v>
       </c>
       <c r="C24">
-        <v>75.400000000000091</v>
+        <v>258</v>
       </c>
       <c r="D24">
-        <v>258</v>
+        <v>398</v>
       </c>
       <c r="E24">
         <v>1.1773147200080301</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>30.845645664210441</v>
+        <v>88.769529888605575</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="1"/>
-        <v>88.769529888605575</v>
+        <v>303.74719776207178</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="2"/>
-        <v>303.74719776207178</v>
+        <v>468.57125856319595</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -2707,28 +2693,28 @@
         <v>2043</v>
       </c>
       <c r="B25">
-        <v>26.799999999999955</v>
+        <v>76.599999999999909</v>
       </c>
       <c r="C25">
-        <v>76.599999999999909</v>
+        <v>262</v>
       </c>
       <c r="D25">
-        <v>262</v>
+        <v>402</v>
       </c>
       <c r="E25">
         <v>1.1773147200080301</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>31.552034496215153</v>
+        <v>90.182307552615001</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="1"/>
-        <v>90.182307552615001</v>
+        <v>308.45645664210389</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="2"/>
-        <v>308.45645664210389</v>
+        <v>473.28051744322806</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -2736,28 +2722,28 @@
         <v>2044</v>
       </c>
       <c r="B26">
-        <v>27.399999999999864</v>
+        <v>77.799999999999727</v>
       </c>
       <c r="C26">
-        <v>77.799999999999727</v>
+        <v>266</v>
       </c>
       <c r="D26">
-        <v>266</v>
+        <v>406</v>
       </c>
       <c r="E26">
         <v>1.1773147200080301</v>
       </c>
       <c r="F26" s="1">
         <f t="shared" si="0"/>
-        <v>32.258423328219862</v>
+        <v>91.595085216624412</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="1"/>
-        <v>91.595085216624412</v>
+        <v>313.165715522136</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="2"/>
-        <v>313.165715522136</v>
+        <v>477.98977632326023</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2765,28 +2751,28 @@
         <v>2045</v>
       </c>
       <c r="B27">
-        <v>28</v>
+        <v>79</v>
       </c>
       <c r="C27">
-        <v>79</v>
+        <v>270</v>
       </c>
       <c r="D27">
-        <v>270</v>
+        <v>410</v>
       </c>
       <c r="E27">
         <v>1.1773147200080301</v>
       </c>
       <c r="F27" s="1">
         <f t="shared" si="0"/>
-        <v>32.964812160224838</v>
+        <v>93.007862880634377</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="1"/>
-        <v>93.007862880634377</v>
+        <v>317.87497440216811</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="2"/>
-        <v>317.87497440216811</v>
+        <v>482.69903520329234</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -2794,28 +2780,28 @@
         <v>2046</v>
       </c>
       <c r="B28">
-        <v>28.800000000000182</v>
+        <v>80.199999999999818</v>
       </c>
       <c r="C28">
-        <v>80.199999999999818</v>
+        <v>274</v>
       </c>
       <c r="D28">
-        <v>274</v>
+        <v>414</v>
       </c>
       <c r="E28">
         <v>1.1773147200080301</v>
       </c>
       <c r="F28" s="1">
         <f t="shared" si="0"/>
-        <v>33.906663936231482</v>
+        <v>94.420640544643803</v>
       </c>
       <c r="G28" s="1">
         <f t="shared" si="1"/>
-        <v>94.420640544643803</v>
+        <v>322.58423328220022</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="2"/>
-        <v>322.58423328220022</v>
+        <v>487.40829408332445</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2823,28 +2809,28 @@
         <v>2047</v>
       </c>
       <c r="B29">
-        <v>29.600000000000136</v>
+        <v>81.400000000000091</v>
       </c>
       <c r="C29">
-        <v>81.400000000000091</v>
+        <v>278</v>
       </c>
       <c r="D29">
-        <v>278</v>
+        <v>418</v>
       </c>
       <c r="E29">
         <v>1.1773147200080301</v>
       </c>
       <c r="F29" s="1">
         <f t="shared" si="0"/>
-        <v>34.848515712237848</v>
+        <v>95.833418208653754</v>
       </c>
       <c r="G29" s="1">
         <f t="shared" si="1"/>
-        <v>95.833418208653754</v>
+        <v>327.29349216223238</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="2"/>
-        <v>327.29349216223238</v>
+        <v>492.11755296335656</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2852,28 +2838,28 @@
         <v>2048</v>
       </c>
       <c r="B30">
-        <v>30.400000000000091</v>
+        <v>82.599999999999909</v>
       </c>
       <c r="C30">
-        <v>82.599999999999909</v>
+        <v>282</v>
       </c>
       <c r="D30">
-        <v>282</v>
+        <v>422</v>
       </c>
       <c r="E30">
         <v>1.1773147200080301</v>
       </c>
       <c r="F30" s="1">
         <f t="shared" si="0"/>
-        <v>35.790367488244222</v>
+        <v>97.246195872663179</v>
       </c>
       <c r="G30" s="1">
         <f t="shared" si="1"/>
-        <v>97.246195872663179</v>
+        <v>332.00275104226449</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="2"/>
-        <v>332.00275104226449</v>
+        <v>496.82681184338867</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2881,28 +2867,28 @@
         <v>2049</v>
       </c>
       <c r="B31">
-        <v>31.200000000000045</v>
+        <v>83.799999999999727</v>
       </c>
       <c r="C31">
-        <v>83.799999999999727</v>
+        <v>286</v>
       </c>
       <c r="D31">
-        <v>286</v>
+        <v>426</v>
       </c>
       <c r="E31">
         <v>1.1773147200080301</v>
       </c>
       <c r="F31" s="1">
         <f t="shared" si="0"/>
-        <v>36.732219264250588</v>
+        <v>98.658973536672605</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="1"/>
-        <v>98.658973536672605</v>
+        <v>336.7120099222966</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="2"/>
-        <v>336.7120099222966</v>
+        <v>501.53607072342078</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2910,28 +2896,28 @@
         <v>2050</v>
       </c>
       <c r="B32">
-        <v>32</v>
+        <v>85</v>
       </c>
       <c r="C32">
-        <v>85</v>
+        <v>290</v>
       </c>
       <c r="D32">
-        <v>290</v>
+        <v>430</v>
       </c>
       <c r="E32">
         <v>1.1773147200080301</v>
       </c>
       <c r="F32" s="1">
         <f t="shared" si="0"/>
-        <v>37.674071040256962</v>
+        <v>100.07175120068256</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="1"/>
-        <v>100.07175120068256</v>
+        <v>341.42126880232871</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="2"/>
-        <v>341.42126880232871</v>
+        <v>506.24532960345294</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed data validation inconsistencies, sanity check on climate and health impact magnitude seems reasonable
</commit_message>
<xml_diff>
--- a/cmu_tare_model/data/marginal_social_costs/scc_climate_impact_sensitivity.xlsx
+++ b/cmu_tare_model/data/marginal_social_costs/scc_climate_impact_sensitivity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\14128\Research\cmu-tare-model\cmu_tare_model\data\marginal_social_costs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A7AA3-D9BE-43A0-B8A4-FE686F117240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C0BF2FD-2D67-41A5-94A7-59019C6073BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{9E84D423-0E0D-4820-8255-FAB67149DDA4}"/>
   </bookViews>
@@ -163,12 +163,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -183,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -191,6 +197,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,8 +369,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6156960" y="762000"/>
-          <a:ext cx="6332769" cy="2270957"/>
+          <a:off x="6159500" y="768773"/>
+          <a:ext cx="6332769" cy="2311597"/>
           <a:chOff x="5913120" y="137160"/>
           <a:chExt cx="6332769" cy="2270957"/>
         </a:xfrm>
@@ -417,7 +424,7 @@
         <xdr:spPr>
           <a:xfrm>
             <a:off x="9174480" y="1005840"/>
-            <a:ext cx="502920" cy="1348740"/>
+            <a:ext cx="502920" cy="868680"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -488,8 +495,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="6156960" y="762000"/>
-          <a:ext cx="6332769" cy="2270957"/>
+          <a:off x="6159500" y="768773"/>
+          <a:ext cx="6332769" cy="2311597"/>
           <a:chOff x="5913120" y="137160"/>
           <a:chExt cx="6332769" cy="2270957"/>
         </a:xfrm>
@@ -542,8 +549,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="9174480" y="1005840"/>
-            <a:ext cx="502920" cy="1348740"/>
+            <a:off x="10919460" y="990600"/>
+            <a:ext cx="502920" cy="876300"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -905,8 +912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75EC15B2-2397-4FE1-8B68-09BFA0B5EF94}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1274,8 +1281,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2851B3AE-E1A0-40CD-8D9C-3E7FD3B3E981}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5754CFF6-6F51-4025-99D4-87B6BEDCE997}">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1977,7 +1984,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2153,15 +2160,15 @@
       <c r="E6">
         <v>1.1773147200080301</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <f t="shared" si="0"/>
         <v>64.752309600441649</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>237.81757344162207</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="5">
         <f t="shared" si="2"/>
         <v>383.80459872261781</v>
       </c>

</xml_diff>